<commit_message>
Updated BOM with caps that are available at this minute, and added 1K parts prices.
</commit_message>
<xml_diff>
--- a/mini/v20/Fubarino_Mini_v20_BOM_Microchip.xlsx
+++ b/mini/v20/Fubarino_Mini_v20_BOM_Microchip.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\fubarino.github.com\mini\v17\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\fubarino.github.com\mini\v20\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C45F8BA-2EF8-465D-AD01-45A3171350BD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E33C7C2-20BB-4956-A9C8-3D1EB44E0F13}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23925" windowHeight="12045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="127">
   <si>
     <t>Approved</t>
   </si>
@@ -177,21 +177,9 @@
     <t>D1, D2</t>
   </si>
   <si>
-    <t>CAP CER 10UF 10V Y5V 0805</t>
-  </si>
-  <si>
-    <t>CAP CERAMIC .100UF 50V X7R 0603</t>
-  </si>
-  <si>
     <t>RES 10K OHM 1/10W 5% 0603 SMD</t>
   </si>
   <si>
-    <t>PIC32 USB CPU</t>
-  </si>
-  <si>
-    <t>CAP CER 12PF 50V 5% NP0 0603</t>
-  </si>
-  <si>
     <t>Microchip</t>
   </si>
   <si>
@@ -204,42 +192,18 @@
     <t>Panasonic</t>
   </si>
   <si>
-    <t>???</t>
-  </si>
-  <si>
-    <t>C2012Y5V1A106Z</t>
-  </si>
-  <si>
-    <t>C0603C104K5RACTU</t>
-  </si>
-  <si>
     <t>ERJ-3GEYJ103V</t>
   </si>
   <si>
-    <t>C0603C120J5GACTU</t>
-  </si>
-  <si>
-    <t>MicrochipDirect</t>
-  </si>
-  <si>
     <t>Diki-Key</t>
   </si>
   <si>
     <t>Brian Schmalz</t>
   </si>
   <si>
-    <t>445-1371-1-ND</t>
-  </si>
-  <si>
-    <t>399-5089-1-ND</t>
-  </si>
-  <si>
     <t>P10KGCT-ND</t>
   </si>
   <si>
-    <t>399-1050-1-ND</t>
-  </si>
-  <si>
     <t>Q2</t>
   </si>
   <si>
@@ -306,9 +270,6 @@
     <t>Parts changed from last production build</t>
   </si>
   <si>
-    <t>PIC32MX270F256D-50I/ML  </t>
-  </si>
-  <si>
     <t>U2</t>
   </si>
   <si>
@@ -393,14 +354,63 @@
     <t>SWITCH TACTILE SPST-NO 0.05A 16V</t>
   </si>
   <si>
-    <t>N</t>
+    <t>Price @1K</t>
+  </si>
+  <si>
+    <t>Total @1K</t>
+  </si>
+  <si>
+    <t>Samsung Electro-Mechanics</t>
+  </si>
+  <si>
+    <t>1276-1052-1-ND</t>
+  </si>
+  <si>
+    <t>CL21A106KPFNNNE</t>
+  </si>
+  <si>
+    <t>CAP CER 10UF 10V X5R 0805</t>
+  </si>
+  <si>
+    <t>311-1343-1-ND</t>
+  </si>
+  <si>
+    <t>Yageo</t>
+  </si>
+  <si>
+    <t>CC0603ZRY5V9BB104</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1UF 50V Y5V 0603</t>
+  </si>
+  <si>
+    <t>PIC32MX270F256D-50I/ML-ND</t>
+  </si>
+  <si>
+    <t>PIC32MX270F256D-50I/ML</t>
+  </si>
+  <si>
+    <t>IC MCU 32BIT 256KB FLASH 44QFN</t>
+  </si>
+  <si>
+    <t>478-7910-1-ND</t>
+  </si>
+  <si>
+    <t>AVX Corporation</t>
+  </si>
+  <si>
+    <t>06035A120GAT2A</t>
+  </si>
+  <si>
+    <t>CAP CER 12PF 50V C0G/NP0 0603</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
@@ -890,7 +900,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
@@ -902,8 +912,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="137">
+  <cellXfs count="151">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -1086,7 +1097,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -1204,33 +1214,6 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1247,8 +1230,78 @@
     <xf numFmtId="0" fontId="17" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="11" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="18" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="18" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="18" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="11" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="3" borderId="8" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="0" fillId="5" borderId="2" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="28" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="10" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="3" fillId="4" borderId="24" xfId="11" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="8" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="8" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="10" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="2" borderId="8" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="2" borderId="10" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="12">
+    <cellStyle name="Currency" xfId="11" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 10" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal 11" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
@@ -1598,30 +1651,32 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M40"/>
+  <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="12.28515625" style="3" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="12.85546875" style="3" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="24.42578125" style="9" customWidth="1"/>
-    <col min="5" max="5" width="37.5703125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="31.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="35" style="3" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" style="3" customWidth="1"/>
     <col min="7" max="7" width="31.28515625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="26.7109375" style="3" customWidth="1"/>
-    <col min="9" max="10" width="28.7109375" style="3" customWidth="1"/>
-    <col min="11" max="11" width="27.28515625" style="3" customWidth="1"/>
-    <col min="12" max="12" width="16" style="3" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="23.42578125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="7.28515625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="7.5703125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="8.42578125" style="133" customWidth="1"/>
     <col min="13" max="13" width="9.140625" style="3" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="3"/>
+    <col min="14" max="15" width="9.140625" style="133"/>
+    <col min="16" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="13.5" thickBot="1">
+    <row r="1" spans="1:15" ht="13.5" thickBot="1">
       <c r="C1" s="32"/>
       <c r="D1" s="33"/>
       <c r="E1" s="34"/>
@@ -1631,16 +1686,16 @@
       <c r="I1" s="34"/>
       <c r="J1" s="34"/>
       <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="62"/>
-    </row>
-    <row r="2" spans="1:13" ht="37.5" customHeight="1" thickBot="1">
+      <c r="L1" s="138"/>
+      <c r="M1" s="61"/>
+    </row>
+    <row r="2" spans="1:15" ht="37.5" customHeight="1" thickBot="1">
       <c r="C2" s="26" t="s">
         <v>19</v>
       </c>
       <c r="D2" s="22"/>
-      <c r="E2" s="77" t="s">
-        <v>104</v>
+      <c r="E2" s="76" t="s">
+        <v>91</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
@@ -1648,15 +1703,15 @@
       <c r="I2" s="56"/>
       <c r="J2" s="56"/>
       <c r="K2" s="56"/>
-      <c r="L2" s="61"/>
-      <c r="M2" s="63"/>
-    </row>
-    <row r="3" spans="1:13" ht="23.25" customHeight="1">
+      <c r="L2" s="139"/>
+      <c r="M2" s="62"/>
+    </row>
+    <row r="3" spans="1:15" ht="23.25" customHeight="1">
       <c r="C3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="74" t="s">
-        <v>84</v>
+      <c r="D3" s="73" t="s">
+        <v>72</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -1664,15 +1719,15 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
-      <c r="K3" s="123"/>
-      <c r="L3" s="120"/>
-      <c r="M3" s="64"/>
-    </row>
-    <row r="4" spans="1:13" ht="17.25" customHeight="1">
+      <c r="K3" s="127"/>
+      <c r="L3" s="140"/>
+      <c r="M3" s="63"/>
+    </row>
+    <row r="4" spans="1:15" ht="17.25" customHeight="1">
       <c r="C4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="75">
+      <c r="D4" s="74">
         <v>2</v>
       </c>
       <c r="E4" s="2"/>
@@ -1681,16 +1736,16 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
-      <c r="K4" s="124"/>
-      <c r="L4" s="121"/>
+      <c r="K4" s="128"/>
+      <c r="L4" s="141"/>
       <c r="M4" s="6"/>
     </row>
-    <row r="5" spans="1:13" ht="17.25" customHeight="1">
+    <row r="5" spans="1:15" ht="17.25" customHeight="1">
       <c r="C5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="76" t="s">
-        <v>67</v>
+      <c r="D5" s="75" t="s">
+        <v>58</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -1698,16 +1753,16 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="124"/>
-      <c r="L5" s="121"/>
+      <c r="K5" s="128"/>
+      <c r="L5" s="141"/>
       <c r="M5" s="6"/>
     </row>
-    <row r="6" spans="1:13" ht="17.25" customHeight="1">
+    <row r="6" spans="1:15" ht="17.25" customHeight="1">
       <c r="C6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="76" t="s">
-        <v>67</v>
+      <c r="D6" s="75" t="s">
+        <v>58</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -1715,11 +1770,11 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="124"/>
-      <c r="L6" s="121"/>
+      <c r="K6" s="128"/>
+      <c r="L6" s="141"/>
       <c r="M6" s="6"/>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:15">
       <c r="C7" s="44"/>
       <c r="D7" s="23"/>
       <c r="E7" s="45"/>
@@ -1727,16 +1782,16 @@
       <c r="G7" s="45"/>
       <c r="H7" s="45"/>
       <c r="I7" s="59"/>
-      <c r="J7" s="85"/>
-      <c r="K7" s="125"/>
-      <c r="L7" s="122"/>
+      <c r="J7" s="84"/>
+      <c r="K7" s="129"/>
+      <c r="L7" s="142"/>
       <c r="M7" s="60"/>
     </row>
-    <row r="8" spans="1:13" ht="15.75" customHeight="1">
+    <row r="8" spans="1:15" ht="15.75" customHeight="1">
       <c r="C8" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="73"/>
+      <c r="D8" s="72"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -1744,14 +1799,14 @@
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="71"/>
-    </row>
-    <row r="9" spans="1:13" ht="15.75" customHeight="1">
+      <c r="L8" s="143"/>
+      <c r="M8" s="70"/>
+    </row>
+    <row r="9" spans="1:15" ht="15.75" customHeight="1">
       <c r="C9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="73"/>
+      <c r="D9" s="72"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -1759,10 +1814,10 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="72"/>
-    </row>
-    <row r="10" spans="1:13" ht="15.75" customHeight="1">
+      <c r="L9" s="143"/>
+      <c r="M9" s="71"/>
+    </row>
+    <row r="10" spans="1:15" ht="15.75" customHeight="1">
       <c r="C10" s="1"/>
       <c r="D10" s="24"/>
       <c r="E10" s="2"/>
@@ -1772,747 +1827,862 @@
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
+      <c r="L10" s="143"/>
       <c r="M10" s="60"/>
     </row>
-    <row r="11" spans="1:13" s="25" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A11" s="78" t="s">
+    <row r="11" spans="1:15" s="25" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A11" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="78" t="s">
+      <c r="B11" s="77" t="s">
         <v>26</v>
       </c>
       <c r="C11" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="79" t="s">
+      <c r="D11" s="78" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="79" t="s">
+      <c r="E11" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="79" t="s">
+      <c r="F11" s="78" t="s">
         <v>30</v>
       </c>
-      <c r="G11" s="79" t="s">
+      <c r="G11" s="78" t="s">
         <v>31</v>
       </c>
-      <c r="H11" s="79" t="s">
+      <c r="H11" s="78" t="s">
         <v>32</v>
       </c>
-      <c r="I11" s="79" t="s">
+      <c r="I11" s="78" t="s">
         <v>34</v>
       </c>
-      <c r="J11" s="86" t="s">
+      <c r="J11" s="85" t="s">
         <v>38</v>
       </c>
-      <c r="K11" s="79" t="s">
+      <c r="K11" s="78" t="s">
         <v>35</v>
       </c>
-      <c r="L11" s="79" t="s">
+      <c r="L11" s="144" t="s">
         <v>36</v>
       </c>
       <c r="M11" s="55" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" s="8" customFormat="1" ht="13.5" thickBot="1">
+      <c r="N11" s="134" t="s">
+        <v>110</v>
+      </c>
+      <c r="O11" s="134" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" s="8" customFormat="1" ht="13.5" thickBot="1">
       <c r="A12" s="8">
         <v>4</v>
       </c>
-      <c r="C12" s="92">
+      <c r="C12" s="91">
         <v>1</v>
       </c>
-      <c r="D12" s="136" t="s">
+      <c r="D12" s="126" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="94" t="s">
-        <v>119</v>
-      </c>
-      <c r="F12" s="93" t="s">
-        <v>117</v>
-      </c>
-      <c r="G12" s="95" t="s">
-        <v>118</v>
-      </c>
-      <c r="H12" s="96" t="s">
+      <c r="E12" s="93" t="s">
+        <v>106</v>
+      </c>
+      <c r="F12" s="92" t="s">
+        <v>104</v>
+      </c>
+      <c r="G12" s="94" t="s">
+        <v>105</v>
+      </c>
+      <c r="H12" s="95" t="s">
         <v>33</v>
       </c>
-      <c r="I12" s="97" t="s">
-        <v>116</v>
-      </c>
-      <c r="J12" s="98" t="s">
+      <c r="I12" s="96" t="s">
+        <v>103</v>
+      </c>
+      <c r="J12" s="97" t="s">
         <v>37</v>
       </c>
-      <c r="K12" s="99">
+      <c r="K12" s="98">
         <v>1</v>
       </c>
-      <c r="L12" s="53">
+      <c r="L12" s="135">
         <v>0.94</v>
       </c>
       <c r="M12" s="54">
         <f t="shared" ref="M12:M29" si="0">K12*L12</f>
         <v>0.94</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" s="8" customFormat="1">
+      <c r="N12" s="135">
+        <v>0.54449999999999998</v>
+      </c>
+      <c r="O12" s="135">
+        <f>C12*N12</f>
+        <v>0.54449999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" s="8" customFormat="1">
       <c r="A13" s="8">
         <v>2</v>
       </c>
-      <c r="C13" s="92">
+      <c r="C13" s="91">
         <v>1</v>
       </c>
-      <c r="D13" s="100" t="s">
-        <v>95</v>
-      </c>
-      <c r="E13" s="129" t="s">
-        <v>96</v>
-      </c>
-      <c r="F13" s="101" t="s">
-        <v>97</v>
-      </c>
-      <c r="G13" s="89" t="s">
-        <v>98</v>
-      </c>
-      <c r="H13" s="96" t="s">
+      <c r="D13" s="99" t="s">
+        <v>82</v>
+      </c>
+      <c r="E13" s="119" t="s">
+        <v>83</v>
+      </c>
+      <c r="F13" s="100" t="s">
+        <v>84</v>
+      </c>
+      <c r="G13" s="88" t="s">
+        <v>85</v>
+      </c>
+      <c r="H13" s="95" t="s">
         <v>33</v>
       </c>
-      <c r="I13" s="90" t="s">
-        <v>99</v>
-      </c>
-      <c r="J13" s="98" t="s">
+      <c r="I13" s="89" t="s">
+        <v>86</v>
+      </c>
+      <c r="J13" s="97" t="s">
         <v>37</v>
       </c>
-      <c r="K13" s="99">
+      <c r="K13" s="98">
         <v>1</v>
       </c>
-      <c r="L13" s="53">
+      <c r="L13" s="135">
         <v>0.45</v>
       </c>
       <c r="M13" s="54">
         <f t="shared" si="0"/>
         <v>0.45</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" s="8" customFormat="1">
+      <c r="N13" s="135">
+        <v>0.12325999999999999</v>
+      </c>
+      <c r="O13" s="135">
+        <f t="shared" ref="O13:O30" si="1">C13*N13</f>
+        <v>0.12325999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" s="8" customFormat="1">
       <c r="A14" s="8">
         <v>1</v>
       </c>
-      <c r="C14" s="92">
+      <c r="C14" s="91">
         <v>1</v>
       </c>
-      <c r="D14" s="100" t="s">
+      <c r="D14" s="99" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="103" t="s">
-        <v>100</v>
-      </c>
-      <c r="F14" s="104" t="s">
-        <v>101</v>
-      </c>
-      <c r="G14" s="105" t="s">
-        <v>102</v>
-      </c>
-      <c r="H14" s="96" t="s">
+      <c r="E14" s="102" t="s">
+        <v>87</v>
+      </c>
+      <c r="F14" s="103" t="s">
+        <v>88</v>
+      </c>
+      <c r="G14" s="104" t="s">
+        <v>89</v>
+      </c>
+      <c r="H14" s="95" t="s">
         <v>33</v>
       </c>
-      <c r="I14" s="106" t="s">
-        <v>103</v>
-      </c>
-      <c r="J14" s="98" t="s">
+      <c r="I14" s="105" t="s">
+        <v>90</v>
+      </c>
+      <c r="J14" s="97" t="s">
         <v>37</v>
       </c>
-      <c r="K14" s="99">
+      <c r="K14" s="98">
         <v>1</v>
       </c>
-      <c r="L14" s="53">
+      <c r="L14" s="135">
         <v>0.56999999999999995</v>
       </c>
       <c r="M14" s="54">
         <f t="shared" si="0"/>
         <v>0.56999999999999995</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" s="8" customFormat="1">
+      <c r="N14" s="135">
+        <v>0.15076999999999999</v>
+      </c>
+      <c r="O14" s="135">
+        <f t="shared" si="1"/>
+        <v>0.15076999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" s="8" customFormat="1">
       <c r="A15" s="8">
         <v>1</v>
       </c>
-      <c r="C15" s="92">
+      <c r="C15" s="91">
         <v>2</v>
       </c>
-      <c r="D15" s="102" t="s">
+      <c r="D15" s="101" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="107" t="s">
-        <v>51</v>
-      </c>
-      <c r="F15" s="104" t="s">
-        <v>57</v>
-      </c>
-      <c r="G15" s="108" t="s">
-        <v>61</v>
-      </c>
-      <c r="H15" s="96" t="s">
+      <c r="E15" s="106" t="s">
+        <v>115</v>
+      </c>
+      <c r="F15" s="103" t="s">
+        <v>112</v>
+      </c>
+      <c r="G15" s="107" t="s">
+        <v>114</v>
+      </c>
+      <c r="H15" s="95" t="s">
         <v>33</v>
       </c>
-      <c r="I15" s="109" t="s">
-        <v>68</v>
-      </c>
-      <c r="J15" s="98" t="s">
+      <c r="I15" s="108" t="s">
+        <v>113</v>
+      </c>
+      <c r="J15" s="97" t="s">
         <v>37</v>
       </c>
-      <c r="K15" s="99">
+      <c r="K15" s="98">
         <v>2</v>
       </c>
-      <c r="L15" s="53">
-        <v>0.15</v>
+      <c r="L15" s="135">
+        <v>0.16</v>
       </c>
       <c r="M15" s="54">
         <f t="shared" si="0"/>
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" s="8" customFormat="1">
+        <v>0.32</v>
+      </c>
+      <c r="N15" s="135">
+        <v>3.1559999999999998E-2</v>
+      </c>
+      <c r="O15" s="135">
+        <f t="shared" si="1"/>
+        <v>6.3119999999999996E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" s="8" customFormat="1">
       <c r="A16" s="8">
         <v>1</v>
       </c>
-      <c r="C16" s="92">
+      <c r="C16" s="91">
         <v>1</v>
       </c>
-      <c r="D16" s="100" t="s">
+      <c r="D16" s="99" t="s">
         <v>42</v>
       </c>
-      <c r="E16" s="103" t="s">
-        <v>108</v>
-      </c>
-      <c r="F16" s="104" t="s">
-        <v>106</v>
-      </c>
-      <c r="G16" s="110" t="s">
-        <v>107</v>
-      </c>
-      <c r="H16" s="96" t="s">
+      <c r="E16" s="102" t="s">
+        <v>95</v>
+      </c>
+      <c r="F16" s="103" t="s">
+        <v>93</v>
+      </c>
+      <c r="G16" s="109" t="s">
+        <v>94</v>
+      </c>
+      <c r="H16" s="95" t="s">
         <v>33</v>
       </c>
-      <c r="I16" s="111" t="s">
-        <v>105</v>
-      </c>
-      <c r="J16" s="98" t="s">
+      <c r="I16" s="110" t="s">
+        <v>92</v>
+      </c>
+      <c r="J16" s="97" t="s">
         <v>37</v>
       </c>
-      <c r="K16" s="99">
+      <c r="K16" s="98">
         <v>1</v>
       </c>
-      <c r="L16" s="53">
+      <c r="L16" s="135">
         <v>0.77</v>
       </c>
       <c r="M16" s="54">
         <f t="shared" si="0"/>
         <v>0.77</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" s="8" customFormat="1">
+      <c r="N16" s="135">
+        <v>0.39929999999999999</v>
+      </c>
+      <c r="O16" s="135">
+        <f t="shared" si="1"/>
+        <v>0.39929999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" s="8" customFormat="1">
       <c r="A17" s="8">
         <v>1</v>
       </c>
-      <c r="C17" s="92">
+      <c r="C17" s="91">
         <v>2</v>
       </c>
-      <c r="D17" s="100" t="s">
+      <c r="D17" s="99" t="s">
         <v>43</v>
       </c>
-      <c r="E17" s="103" t="s">
-        <v>122</v>
-      </c>
-      <c r="F17" s="104" t="s">
-        <v>58</v>
-      </c>
-      <c r="G17" s="105" t="s">
-        <v>121</v>
-      </c>
-      <c r="H17" s="96" t="s">
+      <c r="E17" s="102" t="s">
+        <v>109</v>
+      </c>
+      <c r="F17" s="103" t="s">
+        <v>54</v>
+      </c>
+      <c r="G17" s="104" t="s">
+        <v>108</v>
+      </c>
+      <c r="H17" s="95" t="s">
         <v>33</v>
       </c>
-      <c r="I17" s="106" t="s">
-        <v>120</v>
-      </c>
-      <c r="J17" s="98" t="s">
+      <c r="I17" s="105" t="s">
+        <v>107</v>
+      </c>
+      <c r="J17" s="97" t="s">
         <v>37</v>
       </c>
-      <c r="K17" s="99">
+      <c r="K17" s="98">
         <v>2</v>
       </c>
-      <c r="L17" s="53">
+      <c r="L17" s="135">
         <v>0.3</v>
       </c>
       <c r="M17" s="54">
         <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" s="8" customFormat="1">
+      <c r="N17" s="135">
+        <v>0.17302000000000001</v>
+      </c>
+      <c r="O17" s="135">
+        <f t="shared" si="1"/>
+        <v>0.34604000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" s="8" customFormat="1">
       <c r="A18" s="8">
         <v>1</v>
       </c>
-      <c r="C18" s="92">
+      <c r="C18" s="91">
         <v>4</v>
       </c>
-      <c r="D18" s="102" t="s">
+      <c r="D18" s="101" t="s">
         <v>44</v>
       </c>
-      <c r="E18" s="103" t="s">
-        <v>52</v>
-      </c>
-      <c r="F18" s="104" t="s">
-        <v>57</v>
-      </c>
-      <c r="G18" s="105" t="s">
-        <v>62</v>
-      </c>
-      <c r="H18" s="96" t="s">
+      <c r="E18" s="102" t="s">
+        <v>119</v>
+      </c>
+      <c r="F18" s="103" t="s">
+        <v>117</v>
+      </c>
+      <c r="G18" s="104" t="s">
+        <v>118</v>
+      </c>
+      <c r="H18" s="95" t="s">
         <v>33</v>
       </c>
-      <c r="I18" s="106" t="s">
-        <v>69</v>
-      </c>
-      <c r="J18" s="98" t="s">
+      <c r="I18" s="105" t="s">
+        <v>116</v>
+      </c>
+      <c r="J18" s="97" t="s">
         <v>37</v>
       </c>
-      <c r="K18" s="99">
+      <c r="K18" s="98">
         <v>4</v>
       </c>
-      <c r="L18" s="53" t="s">
-        <v>123</v>
-      </c>
-      <c r="M18" s="54" t="e">
+      <c r="L18" s="135">
+        <v>0.1</v>
+      </c>
+      <c r="M18" s="54">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" s="8" customFormat="1">
+        <v>0.4</v>
+      </c>
+      <c r="N18" s="135">
+        <v>1.541E-2</v>
+      </c>
+      <c r="O18" s="135">
+        <f t="shared" si="1"/>
+        <v>6.164E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" s="8" customFormat="1">
       <c r="A19" s="8">
         <v>2</v>
       </c>
-      <c r="C19" s="92">
+      <c r="C19" s="91">
         <v>1</v>
       </c>
-      <c r="D19" s="100" t="s">
+      <c r="D19" s="99" t="s">
         <v>45</v>
       </c>
-      <c r="E19" s="103" t="s">
-        <v>109</v>
-      </c>
-      <c r="F19" s="104" t="s">
-        <v>110</v>
-      </c>
-      <c r="G19" s="134" t="s">
-        <v>111</v>
-      </c>
-      <c r="H19" s="116" t="s">
+      <c r="E19" s="102" t="s">
+        <v>96</v>
+      </c>
+      <c r="F19" s="103" t="s">
+        <v>97</v>
+      </c>
+      <c r="G19" s="124" t="s">
+        <v>98</v>
+      </c>
+      <c r="H19" s="115" t="s">
         <v>33</v>
       </c>
-      <c r="I19" s="109" t="s">
-        <v>112</v>
-      </c>
-      <c r="J19" s="98" t="s">
+      <c r="I19" s="108" t="s">
+        <v>99</v>
+      </c>
+      <c r="J19" s="97" t="s">
         <v>37</v>
       </c>
-      <c r="K19" s="99">
+      <c r="K19" s="98">
         <v>1</v>
       </c>
-      <c r="L19" s="53">
-        <v>0.15</v>
+      <c r="L19" s="135">
+        <v>0.41</v>
       </c>
       <c r="M19" s="54">
         <f>K19*L19</f>
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" s="8" customFormat="1">
+        <v>0.41</v>
+      </c>
+      <c r="N19" s="135">
+        <v>7.5649999999999995E-2</v>
+      </c>
+      <c r="O19" s="135">
+        <f t="shared" si="1"/>
+        <v>7.5649999999999995E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" s="8" customFormat="1">
       <c r="A20" s="8">
         <v>1</v>
       </c>
-      <c r="C20" s="92">
+      <c r="C20" s="91">
         <v>1</v>
       </c>
-      <c r="D20" s="100" t="s">
+      <c r="D20" s="99" t="s">
         <v>46</v>
       </c>
-      <c r="E20" s="135" t="s">
-        <v>113</v>
-      </c>
-      <c r="F20" s="104" t="s">
-        <v>110</v>
-      </c>
-      <c r="G20" s="130" t="s">
-        <v>114</v>
-      </c>
-      <c r="H20" s="96" t="s">
+      <c r="E20" s="125" t="s">
+        <v>100</v>
+      </c>
+      <c r="F20" s="103" t="s">
+        <v>97</v>
+      </c>
+      <c r="G20" s="120" t="s">
+        <v>101</v>
+      </c>
+      <c r="H20" s="95" t="s">
         <v>33</v>
       </c>
-      <c r="I20" s="135" t="s">
-        <v>115</v>
-      </c>
-      <c r="J20" s="98" t="s">
+      <c r="I20" s="125" t="s">
+        <v>102</v>
+      </c>
+      <c r="J20" s="97" t="s">
         <v>37</v>
       </c>
-      <c r="K20" s="99">
+      <c r="K20" s="98">
         <v>1</v>
       </c>
-      <c r="L20" s="53">
-        <v>0.15</v>
+      <c r="L20" s="135">
+        <v>0.41</v>
       </c>
       <c r="M20" s="54">
         <f t="shared" si="0"/>
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" s="8" customFormat="1">
+        <v>0.41</v>
+      </c>
+      <c r="N20" s="135">
+        <v>7.5649999999999995E-2</v>
+      </c>
+      <c r="O20" s="135">
+        <f t="shared" si="1"/>
+        <v>7.5649999999999995E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" s="8" customFormat="1">
       <c r="A21" s="8">
         <v>2</v>
       </c>
-      <c r="C21" s="92">
+      <c r="C21" s="91">
         <v>2</v>
       </c>
-      <c r="D21" s="100" t="s">
+      <c r="D21" s="99" t="s">
         <v>47</v>
       </c>
-      <c r="E21" s="103" t="s">
-        <v>85</v>
-      </c>
-      <c r="F21" s="104" t="s">
-        <v>59</v>
-      </c>
-      <c r="G21" s="105" t="s">
-        <v>86</v>
-      </c>
-      <c r="H21" s="96" t="s">
+      <c r="E21" s="102" t="s">
+        <v>73</v>
+      </c>
+      <c r="F21" s="103" t="s">
+        <v>55</v>
+      </c>
+      <c r="G21" s="104" t="s">
+        <v>74</v>
+      </c>
+      <c r="H21" s="95" t="s">
         <v>33</v>
       </c>
-      <c r="I21" s="90" t="s">
-        <v>87</v>
-      </c>
-      <c r="J21" s="98" t="s">
+      <c r="I21" s="89" t="s">
+        <v>75</v>
+      </c>
+      <c r="J21" s="97" t="s">
         <v>37</v>
       </c>
-      <c r="K21" s="99">
+      <c r="K21" s="98">
         <v>2</v>
       </c>
-      <c r="L21" s="53">
+      <c r="L21" s="135">
         <v>0.1</v>
       </c>
       <c r="M21" s="54">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" s="8" customFormat="1">
+      <c r="N21" s="135">
+        <v>8.5800000000000008E-3</v>
+      </c>
+      <c r="O21" s="135">
+        <f t="shared" si="1"/>
+        <v>1.7160000000000002E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" s="8" customFormat="1">
       <c r="A22" s="8">
         <v>1</v>
       </c>
-      <c r="C22" s="92">
+      <c r="C22" s="91">
         <v>3</v>
       </c>
-      <c r="D22" s="102" t="s">
+      <c r="D22" s="101" t="s">
         <v>48</v>
       </c>
-      <c r="E22" s="103" t="s">
-        <v>53</v>
-      </c>
-      <c r="F22" s="104" t="s">
+      <c r="E22" s="102" t="s">
+        <v>51</v>
+      </c>
+      <c r="F22" s="103" t="s">
+        <v>55</v>
+      </c>
+      <c r="G22" s="104" t="s">
+        <v>56</v>
+      </c>
+      <c r="H22" s="95" t="s">
+        <v>33</v>
+      </c>
+      <c r="I22" s="105" t="s">
         <v>59</v>
       </c>
-      <c r="G22" s="105" t="s">
-        <v>63</v>
-      </c>
-      <c r="H22" s="96" t="s">
-        <v>33</v>
-      </c>
-      <c r="I22" s="106" t="s">
-        <v>70</v>
-      </c>
-      <c r="J22" s="98" t="s">
+      <c r="J22" s="97" t="s">
         <v>37</v>
       </c>
-      <c r="K22" s="99">
+      <c r="K22" s="98">
         <v>3</v>
       </c>
-      <c r="L22" s="53">
+      <c r="L22" s="135">
         <v>0.1</v>
       </c>
       <c r="M22" s="54">
         <f t="shared" si="0"/>
         <v>0.30000000000000004</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" s="8" customFormat="1">
+      <c r="N22" s="135">
+        <v>8.5800000000000008E-3</v>
+      </c>
+      <c r="O22" s="135">
+        <f t="shared" si="1"/>
+        <v>2.5740000000000002E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" s="8" customFormat="1">
       <c r="A23" s="8">
         <v>4</v>
       </c>
-      <c r="C23" s="92">
+      <c r="C23" s="91">
         <v>1</v>
       </c>
-      <c r="D23" s="100" t="s">
+      <c r="D23" s="99" t="s">
         <v>28</v>
       </c>
-      <c r="E23" s="103" t="s">
-        <v>54</v>
-      </c>
-      <c r="F23" s="104" t="s">
-        <v>56</v>
-      </c>
-      <c r="G23" s="133" t="s">
-        <v>94</v>
-      </c>
-      <c r="H23" s="96" t="s">
-        <v>65</v>
-      </c>
-      <c r="I23" s="119" t="s">
-        <v>94</v>
-      </c>
-      <c r="J23" s="98" t="s">
+      <c r="E23" s="102" t="s">
+        <v>122</v>
+      </c>
+      <c r="F23" s="103" t="s">
+        <v>52</v>
+      </c>
+      <c r="G23" s="123" t="s">
+        <v>121</v>
+      </c>
+      <c r="H23" s="95" t="s">
+        <v>33</v>
+      </c>
+      <c r="I23" s="118" t="s">
+        <v>120</v>
+      </c>
+      <c r="J23" s="97" t="s">
         <v>37</v>
       </c>
-      <c r="K23" s="99">
+      <c r="K23" s="98">
         <v>1</v>
       </c>
-      <c r="L23" s="53">
-        <v>4.49</v>
+      <c r="L23" s="135">
+        <v>4.62</v>
       </c>
       <c r="M23" s="54">
         <f t="shared" si="0"/>
-        <v>4.49</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" s="8" customFormat="1">
+        <v>4.62</v>
+      </c>
+      <c r="N23" s="135">
+        <v>3.8418999999999999</v>
+      </c>
+      <c r="O23" s="135">
+        <f t="shared" si="1"/>
+        <v>3.8418999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" s="8" customFormat="1">
       <c r="A24" s="8">
         <v>1</v>
       </c>
-      <c r="C24" s="92">
+      <c r="C24" s="91">
         <v>2</v>
       </c>
-      <c r="D24" s="102" t="s">
+      <c r="D24" s="101" t="s">
         <v>49</v>
       </c>
-      <c r="E24" s="112" t="s">
-        <v>55</v>
-      </c>
-      <c r="F24" s="131" t="s">
-        <v>57</v>
-      </c>
-      <c r="G24" s="113" t="s">
-        <v>64</v>
-      </c>
-      <c r="H24" s="132" t="s">
+      <c r="E24" s="111" t="s">
+        <v>126</v>
+      </c>
+      <c r="F24" s="121" t="s">
+        <v>124</v>
+      </c>
+      <c r="G24" s="112" t="s">
+        <v>125</v>
+      </c>
+      <c r="H24" s="122" t="s">
         <v>33</v>
       </c>
-      <c r="I24" s="114" t="s">
-        <v>71</v>
-      </c>
-      <c r="J24" s="98" t="s">
+      <c r="I24" s="113" t="s">
+        <v>123</v>
+      </c>
+      <c r="J24" s="97" t="s">
         <v>37</v>
       </c>
-      <c r="K24" s="99">
+      <c r="K24" s="98">
         <v>2</v>
       </c>
-      <c r="L24" s="53">
-        <v>0.1</v>
+      <c r="L24" s="135">
+        <v>0.52</v>
       </c>
       <c r="M24" s="54">
         <f t="shared" si="0"/>
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" s="8" customFormat="1">
+        <v>1.04</v>
+      </c>
+      <c r="N24" s="135">
+        <v>0.13650000000000001</v>
+      </c>
+      <c r="O24" s="135">
+        <f t="shared" si="1"/>
+        <v>0.27300000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" s="8" customFormat="1">
       <c r="A25" s="8">
         <v>1</v>
       </c>
-      <c r="C25" s="92">
+      <c r="C25" s="91">
         <v>1</v>
       </c>
-      <c r="D25" s="115"/>
-      <c r="E25" s="103" t="s">
-        <v>88</v>
-      </c>
-      <c r="F25" s="104" t="s">
-        <v>60</v>
-      </c>
-      <c r="G25" s="108" t="s">
-        <v>60</v>
-      </c>
-      <c r="H25" s="116" t="s">
-        <v>60</v>
-      </c>
-      <c r="I25" s="109" t="s">
-        <v>60</v>
-      </c>
-      <c r="J25" s="98" t="s">
+      <c r="D25" s="114"/>
+      <c r="E25" s="102" t="s">
+        <v>76</v>
+      </c>
+      <c r="F25" s="103"/>
+      <c r="G25" s="107"/>
+      <c r="H25" s="115"/>
+      <c r="I25" s="108"/>
+      <c r="J25" s="97" t="s">
         <v>37</v>
       </c>
-      <c r="K25" s="99">
+      <c r="K25" s="98">
         <v>1</v>
       </c>
-      <c r="L25" s="53"/>
+      <c r="L25" s="135"/>
       <c r="M25" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" s="8" customFormat="1">
+      <c r="N25" s="135"/>
+      <c r="O25" s="135">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" s="8" customFormat="1">
       <c r="A26" s="8">
         <v>2</v>
       </c>
-      <c r="C26" s="92">
+      <c r="C26" s="91">
         <v>2</v>
       </c>
-      <c r="D26" s="100" t="s">
+      <c r="D26" s="99" t="s">
         <v>50</v>
       </c>
-      <c r="E26" s="112" t="s">
-        <v>91</v>
-      </c>
-      <c r="F26" s="101" t="s">
-        <v>92</v>
-      </c>
-      <c r="G26" s="130" t="s">
-        <v>89</v>
-      </c>
-      <c r="H26" s="96" t="s">
-        <v>66</v>
-      </c>
-      <c r="I26" s="90" t="s">
-        <v>90</v>
-      </c>
-      <c r="J26" s="98" t="s">
+      <c r="E26" s="111" t="s">
+        <v>79</v>
+      </c>
+      <c r="F26" s="100" t="s">
+        <v>80</v>
+      </c>
+      <c r="G26" s="120" t="s">
+        <v>77</v>
+      </c>
+      <c r="H26" s="95" t="s">
+        <v>57</v>
+      </c>
+      <c r="I26" s="89" t="s">
+        <v>78</v>
+      </c>
+      <c r="J26" s="97" t="s">
         <v>37</v>
       </c>
-      <c r="K26" s="99">
+      <c r="K26" s="98">
         <v>2</v>
       </c>
-      <c r="L26" s="53">
+      <c r="L26" s="135">
         <v>0.47</v>
       </c>
       <c r="M26" s="54">
         <f t="shared" si="0"/>
         <v>0.94</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" s="8" customFormat="1">
+      <c r="N26" s="135">
+        <v>8.7059999999999998E-2</v>
+      </c>
+      <c r="O26" s="135">
+        <f t="shared" si="1"/>
+        <v>0.17412</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" s="8" customFormat="1">
       <c r="A27" s="8">
         <v>1</v>
       </c>
-      <c r="C27" s="126" t="s">
-        <v>83</v>
-      </c>
-      <c r="D27" s="127"/>
-      <c r="E27" s="127"/>
-      <c r="F27" s="127"/>
-      <c r="G27" s="128"/>
-      <c r="H27" s="117"/>
-      <c r="I27" s="117"/>
-      <c r="J27" s="98"/>
-      <c r="K27" s="98"/>
-      <c r="L27" s="53"/>
+      <c r="C27" s="130" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27" s="131"/>
+      <c r="E27" s="131"/>
+      <c r="F27" s="131"/>
+      <c r="G27" s="132"/>
+      <c r="H27" s="116"/>
+      <c r="I27" s="116"/>
+      <c r="J27" s="97"/>
+      <c r="K27" s="97"/>
+      <c r="L27" s="135"/>
       <c r="M27" s="54"/>
-    </row>
-    <row r="28" spans="1:13" s="8" customFormat="1">
-      <c r="C28" s="92">
+      <c r="N27" s="135"/>
+      <c r="O27" s="135"/>
+    </row>
+    <row r="28" spans="1:15" s="8" customFormat="1">
+      <c r="C28" s="91">
         <v>0</v>
       </c>
-      <c r="D28" s="93" t="s">
-        <v>72</v>
-      </c>
-      <c r="E28" s="118" t="s">
-        <v>75</v>
-      </c>
-      <c r="F28" s="104" t="s">
-        <v>78</v>
-      </c>
-      <c r="G28" s="118" t="s">
-        <v>79</v>
-      </c>
-      <c r="H28" s="118" t="s">
+      <c r="D28" s="92" t="s">
+        <v>60</v>
+      </c>
+      <c r="E28" s="117" t="s">
+        <v>63</v>
+      </c>
+      <c r="F28" s="103" t="s">
+        <v>66</v>
+      </c>
+      <c r="G28" s="117" t="s">
+        <v>67</v>
+      </c>
+      <c r="H28" s="117" t="s">
         <v>33</v>
       </c>
-      <c r="I28" s="118" t="s">
-        <v>81</v>
-      </c>
-      <c r="J28" s="98" t="s">
+      <c r="I28" s="117" t="s">
+        <v>69</v>
+      </c>
+      <c r="J28" s="97" t="s">
         <v>37</v>
       </c>
-      <c r="K28" s="98">
+      <c r="K28" s="97">
         <v>0</v>
       </c>
-      <c r="L28" s="53">
+      <c r="L28" s="135">
         <v>0.3</v>
       </c>
       <c r="M28" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" s="8" customFormat="1">
+      <c r="N28" s="135"/>
+      <c r="O28" s="135">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" s="8" customFormat="1">
       <c r="A29" s="8">
         <v>1</v>
       </c>
-      <c r="C29" s="92">
+      <c r="C29" s="91">
         <v>0</v>
       </c>
-      <c r="D29" s="93" t="s">
-        <v>73</v>
-      </c>
-      <c r="E29" s="101" t="s">
-        <v>76</v>
-      </c>
-      <c r="F29" s="104" t="s">
-        <v>57</v>
-      </c>
-      <c r="G29" s="101" t="s">
-        <v>80</v>
-      </c>
-      <c r="H29" s="101" t="s">
+      <c r="D29" s="92" t="s">
+        <v>61</v>
+      </c>
+      <c r="E29" s="100" t="s">
+        <v>64</v>
+      </c>
+      <c r="F29" s="103" t="s">
+        <v>53</v>
+      </c>
+      <c r="G29" s="100" t="s">
+        <v>68</v>
+      </c>
+      <c r="H29" s="100" t="s">
         <v>33</v>
       </c>
-      <c r="I29" s="101" t="s">
-        <v>82</v>
-      </c>
-      <c r="J29" s="98" t="s">
+      <c r="I29" s="100" t="s">
+        <v>70</v>
+      </c>
+      <c r="J29" s="97" t="s">
         <v>37</v>
       </c>
-      <c r="K29" s="98">
+      <c r="K29" s="97">
         <v>0</v>
       </c>
-      <c r="L29" s="53">
+      <c r="L29" s="135">
         <v>0.1</v>
       </c>
       <c r="M29" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" s="8" customFormat="1">
+      <c r="N29" s="135"/>
+      <c r="O29" s="135">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" s="8" customFormat="1">
       <c r="A30" s="8">
         <v>1</v>
       </c>
       <c r="C30" s="58">
         <v>0</v>
       </c>
-      <c r="D30" s="87" t="s">
-        <v>74</v>
-      </c>
-      <c r="E30" s="88" t="s">
-        <v>77</v>
-      </c>
-      <c r="F30" s="80"/>
-      <c r="G30" s="80"/>
-      <c r="H30" s="80"/>
-      <c r="I30" s="80"/>
+      <c r="D30" s="86" t="s">
+        <v>62</v>
+      </c>
+      <c r="E30" s="87" t="s">
+        <v>65</v>
+      </c>
+      <c r="F30" s="79"/>
+      <c r="G30" s="79"/>
+      <c r="H30" s="79"/>
+      <c r="I30" s="79"/>
       <c r="J30" s="53"/>
       <c r="K30" s="53"/>
-      <c r="L30" s="53"/>
+      <c r="L30" s="135"/>
       <c r="M30" s="54"/>
-    </row>
-    <row r="31" spans="1:13">
+      <c r="N30" s="135"/>
+      <c r="O30" s="135"/>
+    </row>
+    <row r="31" spans="1:15">
       <c r="C31" s="48"/>
       <c r="D31" s="49"/>
       <c r="E31" s="49"/>
@@ -2522,13 +2692,18 @@
       <c r="I31" s="50"/>
       <c r="J31" s="50"/>
       <c r="K31" s="50"/>
-      <c r="L31" s="50"/>
-      <c r="M31" s="52" t="e">
+      <c r="L31" s="145"/>
+      <c r="M31" s="52">
         <f>SUM(M12:M30)</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" customFormat="1" ht="13.7" customHeight="1">
+        <v>11.97</v>
+      </c>
+      <c r="N31" s="136"/>
+      <c r="O31" s="136">
+        <f>SUM(O12:O29)</f>
+        <v>6.1718499999999992</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" customFormat="1" ht="13.7" customHeight="1">
       <c r="C32" s="35" t="s">
         <v>0</v>
       </c>
@@ -2542,12 +2717,14 @@
       <c r="I32" s="47"/>
       <c r="J32" s="47"/>
       <c r="K32" s="47"/>
-      <c r="L32" s="27"/>
+      <c r="L32" s="146"/>
       <c r="M32" s="41" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="33" spans="3:13" customFormat="1" ht="12.95" customHeight="1">
+      <c r="N32" s="137"/>
+      <c r="O32" s="137"/>
+    </row>
+    <row r="33" spans="3:15" customFormat="1" ht="12.95" customHeight="1">
       <c r="C33" s="38"/>
       <c r="D33" s="39"/>
       <c r="E33" s="40"/>
@@ -2557,14 +2734,16 @@
       <c r="I33" s="51"/>
       <c r="J33" s="51"/>
       <c r="K33" s="51"/>
-      <c r="L33" s="51"/>
-      <c r="M33" s="68"/>
-    </row>
-    <row r="34" spans="3:13" customFormat="1" ht="12.95" customHeight="1">
+      <c r="L33" s="147"/>
+      <c r="M33" s="67"/>
+      <c r="N33" s="137"/>
+      <c r="O33" s="137"/>
+    </row>
+    <row r="34" spans="3:15" customFormat="1" ht="12.95" customHeight="1">
       <c r="C34" s="36"/>
       <c r="D34" s="30"/>
-      <c r="E34" s="91" t="s">
-        <v>93</v>
+      <c r="E34" s="90" t="s">
+        <v>81</v>
       </c>
       <c r="F34" s="27"/>
       <c r="G34" s="27"/>
@@ -2572,10 +2751,12 @@
       <c r="I34" s="27"/>
       <c r="J34" s="27"/>
       <c r="K34" s="27"/>
-      <c r="L34" s="27"/>
-      <c r="M34" s="69"/>
-    </row>
-    <row r="35" spans="3:13" customFormat="1" ht="12.95" customHeight="1">
+      <c r="L34" s="146"/>
+      <c r="M34" s="68"/>
+      <c r="N34" s="137"/>
+      <c r="O34" s="137"/>
+    </row>
+    <row r="35" spans="3:15" customFormat="1" ht="12.95" customHeight="1">
       <c r="C35" s="36"/>
       <c r="D35" s="30"/>
       <c r="E35" s="31"/>
@@ -2585,10 +2766,12 @@
       <c r="I35" s="27"/>
       <c r="J35" s="27"/>
       <c r="K35" s="27"/>
-      <c r="L35" s="27"/>
-      <c r="M35" s="69"/>
-    </row>
-    <row r="36" spans="3:13" customFormat="1" ht="12.95" customHeight="1">
+      <c r="L35" s="146"/>
+      <c r="M35" s="68"/>
+      <c r="N35" s="137"/>
+      <c r="O35" s="137"/>
+    </row>
+    <row r="36" spans="3:15" customFormat="1" ht="12.95" customHeight="1">
       <c r="C36" s="36"/>
       <c r="D36" s="30"/>
       <c r="E36" s="31"/>
@@ -2598,10 +2781,12 @@
       <c r="I36" s="27"/>
       <c r="J36" s="27"/>
       <c r="K36" s="27"/>
-      <c r="L36" s="27"/>
-      <c r="M36" s="69"/>
-    </row>
-    <row r="37" spans="3:13" customFormat="1" ht="9.75" customHeight="1">
+      <c r="L36" s="146"/>
+      <c r="M36" s="68"/>
+      <c r="N36" s="137"/>
+      <c r="O36" s="137"/>
+    </row>
+    <row r="37" spans="3:15" customFormat="1" ht="9.75" customHeight="1">
       <c r="C37" s="37"/>
       <c r="D37" s="42"/>
       <c r="E37" s="43"/>
@@ -2611,10 +2796,12 @@
       <c r="I37" s="29"/>
       <c r="J37" s="29"/>
       <c r="K37" s="29"/>
-      <c r="L37" s="29"/>
-      <c r="M37" s="70"/>
-    </row>
-    <row r="38" spans="3:13" customFormat="1" ht="12.95" customHeight="1">
+      <c r="L37" s="148"/>
+      <c r="M37" s="69"/>
+      <c r="N37" s="137"/>
+      <c r="O37" s="137"/>
+    </row>
+    <row r="38" spans="3:15" customFormat="1" ht="12.95" customHeight="1">
       <c r="C38" s="37"/>
       <c r="D38" s="28"/>
       <c r="E38" s="29"/>
@@ -2624,10 +2811,12 @@
       <c r="I38" s="29"/>
       <c r="J38" s="29"/>
       <c r="K38" s="29"/>
-      <c r="L38" s="29"/>
-      <c r="M38" s="67"/>
-    </row>
-    <row r="39" spans="3:13" customFormat="1" ht="12.95" customHeight="1">
+      <c r="L38" s="148"/>
+      <c r="M38" s="66"/>
+      <c r="N38" s="137"/>
+      <c r="O38" s="137"/>
+    </row>
+    <row r="39" spans="3:15" customFormat="1" ht="12.95" customHeight="1">
       <c r="C39" s="16"/>
       <c r="D39" s="17"/>
       <c r="E39" s="18"/>
@@ -2637,10 +2826,12 @@
       <c r="I39" s="18"/>
       <c r="J39" s="18"/>
       <c r="K39" s="18"/>
-      <c r="L39" s="18"/>
-      <c r="M39" s="65"/>
-    </row>
-    <row r="40" spans="3:13" customFormat="1" ht="12.95" customHeight="1">
+      <c r="L39" s="149"/>
+      <c r="M39" s="64"/>
+      <c r="N39" s="137"/>
+      <c r="O39" s="137"/>
+    </row>
+    <row r="40" spans="3:15" customFormat="1" ht="12.95" customHeight="1">
       <c r="C40" s="19"/>
       <c r="D40" s="20"/>
       <c r="E40" s="21"/>
@@ -2650,8 +2841,10 @@
       <c r="I40" s="21"/>
       <c r="J40" s="21"/>
       <c r="K40" s="21"/>
-      <c r="L40" s="21"/>
-      <c r="M40" s="66"/>
+      <c r="L40" s="150"/>
+      <c r="M40" s="65"/>
+      <c r="N40" s="137"/>
+      <c r="O40" s="137"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2686,85 +2879,85 @@
       <c r="A1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="81"/>
+      <c r="B1" s="80"/>
     </row>
     <row r="2" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1">
       <c r="A2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="82"/>
+      <c r="B2" s="81"/>
     </row>
     <row r="3" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1">
       <c r="A3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="83"/>
+      <c r="B3" s="82"/>
     </row>
     <row r="4" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1">
       <c r="A4" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="82"/>
+      <c r="B4" s="81"/>
     </row>
     <row r="5" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1">
       <c r="A5" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="83"/>
+      <c r="B5" s="82"/>
     </row>
     <row r="6" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1">
       <c r="A6" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="82"/>
+      <c r="B6" s="81"/>
     </row>
     <row r="7" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1">
       <c r="A7" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="83"/>
+      <c r="B7" s="82"/>
     </row>
     <row r="8" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1">
       <c r="A8" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="82"/>
+      <c r="B8" s="81"/>
     </row>
     <row r="9" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="83"/>
+      <c r="B9" s="82"/>
     </row>
     <row r="10" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1">
       <c r="A10" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="82"/>
+      <c r="B10" s="81"/>
     </row>
     <row r="11" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1">
       <c r="A11" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="83"/>
+      <c r="B11" s="82"/>
     </row>
     <row r="12" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1">
       <c r="A12" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="82"/>
+      <c r="B12" s="81"/>
     </row>
     <row r="13" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1">
       <c r="A13" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="83"/>
+      <c r="B13" s="82"/>
     </row>
     <row r="14" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" thickBot="1">
       <c r="A14" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="84"/>
+      <c r="B14" s="83"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>

</xml_diff>